<commit_message>
latest updates from MVP branch in Rappi_Scrapper + output.cvs working
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="address" state="visible" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
   <si>
     <t>Address</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>sabao em po</t>
+  </si>
+  <si>
+    <t>detergente</t>
+  </si>
+  <si>
+    <t>Sabao em po</t>
   </si>
   <si>
     <t>Detergente</t>
@@ -547,7 +556,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1049"/>
+  <dimension ref="A1:A1051"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2"/>
@@ -586,132 +595,132 @@
     </row>
     <row r="6" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -721,161 +730,169 @@
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="53" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="54" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="55" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="56" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="62" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1854,6 +1871,8 @@
     <row r="1047" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1048" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1049" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1050" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1051" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -1868,7 +1887,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="14.44140625" customHeight="1"/>
@@ -1888,22 +1907,13 @@
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>query!A3</f>
-        <v>cafe forte</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>query!A4</f>
-        <v>cafe extra forte</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>query!A5</f>
-        <v>cafe extra forte</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2896,7 +2906,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1049"/>
+  <dimension ref="A1:A1053"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2"/>
@@ -2930,27 +2940,27 @@
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2970,37 +2980,37 @@
     </row>
     <row r="13" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3015,7 +3025,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3030,203 +3040,219 @@
     </row>
     <row r="25" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>53</v>
+      <c r="A51" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="52" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A52" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="53" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="54" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="58" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4203,6 +4229,10 @@
     <row r="1047" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1048" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1049" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1050" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1051" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1052" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1053" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4228,37 +4258,37 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>